<commit_message>
updated BB_recipe_bounds with Stretch Mins
</commit_message>
<xml_diff>
--- a/data/BB_recipe_bounds.xlsx
+++ b/data/BB_recipe_bounds.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29721"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="98" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96046465-985A-4890-AA17-B195A46BB78E}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C2E1D50-03C1-4A5E-96A7-524263B0B8A5}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
   <si>
     <t>this file is used in the BB optimizer python code. DO NOT CHANGE anything in here unless it is done in accordance with code changes.</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Absolute Max</t>
+  </si>
+  <si>
+    <t>Stretch Min</t>
   </si>
   <si>
     <t>Notes</t>
@@ -487,10 +490,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="G4" sqref="G4:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -498,7 +501,7 @@
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="30.75">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="30.75">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -520,10 +523,13 @@
       <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>5</v>
@@ -541,9 +547,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>9.75</v>
@@ -561,9 +567,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4">
         <v>2</v>
@@ -580,10 +586,13 @@
       <c r="F4" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4">
         <v>2.5</v>
@@ -600,10 +609,13 @@
       <c r="F5" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4">
         <v>2</v>
@@ -620,10 +632,13 @@
       <c r="F6" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4">
         <v>3.75</v>
@@ -640,8 +655,11 @@
       <c r="F7" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="B8" s="6">
         <f>SUM(B2:B7)</f>
         <v>25</v>
@@ -654,10 +672,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD644C8-0F08-481C-9A2D-47BC14CF6CBE}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="G4" sqref="G4:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -665,7 +683,7 @@
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="30.75">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="30.75">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -687,10 +705,13 @@
       <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>3</v>
@@ -708,9 +729,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>10.75</v>
@@ -728,9 +749,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4">
         <v>2.5</v>
@@ -747,10 +768,13 @@
       <c r="F4" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4">
         <v>2.5</v>
@@ -767,10 +791,13 @@
       <c r="F5" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4">
         <v>2.5</v>
@@ -787,10 +814,13 @@
       <c r="F6" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4">
         <v>3.75</v>
@@ -807,8 +837,11 @@
       <c r="F7" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="B8" s="6">
         <f>SUM(B2:B7)</f>
         <v>25</v>
@@ -821,15 +854,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DBA16F4-0378-47F3-910D-C41B503DF6B3}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="30.75">
+    <row r="1" spans="1:8" ht="30.75">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -851,10 +884,13 @@
       <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>8.25</v>
@@ -872,9 +908,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>5</v>
@@ -892,9 +928,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4">
         <v>2.5</v>
@@ -911,10 +947,13 @@
       <c r="F4" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4">
         <v>2.75</v>
@@ -931,10 +970,13 @@
       <c r="F5" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4">
         <v>2.75</v>
@@ -951,10 +993,13 @@
       <c r="F6" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4">
         <v>3.75</v>
@@ -971,8 +1016,11 @@
       <c r="F7" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="B8" s="6">
         <f>SUM(B2:B7)</f>
         <v>25</v>

</xml_diff>

<commit_message>
changed design max of focals in late spring. existing number seemed way too high
</commit_message>
<xml_diff>
--- a/data/BB_recipe_bounds.xlsx
+++ b/data/BB_recipe_bounds.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10201"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="114" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C2E1D50-03C1-4A5E-96A7-524263B0B8A5}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharon/Documents/Sweet Piedmont/Offerings/Software and Code/bouquet-blueprint-app/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC2FBDC-AF2F-8E45-9D0A-38ACB83D358C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="760" windowWidth="14800" windowHeight="8020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="4" r:id="rId1"/>
@@ -88,7 +93,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,9 +171,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -206,7 +211,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -312,7 +317,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -454,7 +459,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -468,17 +473,17 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="76.5703125" customWidth="1"/>
+    <col min="1" max="1" width="76.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="30.75">
+    <row r="1" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="45.75">
+    <row r="3" spans="1:1" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -496,12 +501,12 @@
       <selection activeCell="G4" sqref="G4:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="30.75">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -527,7 +532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -547,7 +552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -567,7 +572,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -590,7 +595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -613,7 +618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -636,7 +641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -659,7 +664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="6">
         <f>SUM(B2:B7)</f>
         <v>25</v>
@@ -674,16 +679,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD644C8-0F08-481C-9A2D-47BC14CF6CBE}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="30.75">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -709,7 +714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -720,7 +725,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2" s="4">
         <v>1</v>
@@ -729,7 +734,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -749,7 +754,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -772,7 +777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -795,7 +800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -818,7 +823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -841,7 +846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="6">
         <f>SUM(B2:B7)</f>
         <v>25</v>
@@ -856,13 +861,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DBA16F4-0378-47F3-910D-C41B503DF6B3}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.75">
+    <row r="1" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -888,7 +893,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -908,7 +913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -928,7 +933,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -951,7 +956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -974,7 +979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -997,7 +1002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1020,7 +1025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="6">
         <f>SUM(B2:B7)</f>
         <v>25</v>

</xml_diff>